<commit_message>
1. converted default unit init in mechanisms to rely on a json file rather than static typing. 2. slight modifications to mechanisms, models, and metadata to pass unit tests
</commit_message>
<xml_diff>
--- a/test/test_database.xlsx
+++ b/test/test_database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MT_RESEARCH/2D_Petrology/mineral_conductivity/mineralconductivities/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/X9 Pro/Recovered Data  - EXFAT/MT_RESEARCH/2D_Petrology/mineral_conductivity/mineralconductivities/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2944CF35-68EA-154C-A31F-2B46EFF7163D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{673E85B5-CA5F-B748-8F67-8DF124AB6D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16720" xr2:uid="{EF1EAB3C-7106-8347-9382-DA47A6680CFD}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16680" xr2:uid="{EF1EAB3C-7106-8347-9382-DA47A6680CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="test_database" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="635" uniqueCount="206">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="647" uniqueCount="218">
   <si>
     <t>Title</t>
   </si>
@@ -657,6 +657,42 @@
   </si>
   <si>
     <t>arrhenious_simple+arrhenious_simple</t>
+  </si>
+  <si>
+    <t>Na2o Min</t>
+  </si>
+  <si>
+    <t>Na2o Max</t>
+  </si>
+  <si>
+    <t>SiO2 Max</t>
+  </si>
+  <si>
+    <t>Na2O Average</t>
+  </si>
+  <si>
+    <t>SiO2 Min</t>
+  </si>
+  <si>
+    <t>NaCl Min</t>
+  </si>
+  <si>
+    <t>NaCl Max</t>
+  </si>
+  <si>
+    <t>NaCl Average</t>
+  </si>
+  <si>
+    <t>SiO2 Average</t>
+  </si>
+  <si>
+    <t>CO2 min</t>
+  </si>
+  <si>
+    <t>CO2 max</t>
+  </si>
+  <si>
+    <t>CO2 average</t>
   </si>
 </sst>
 </file>
@@ -776,9 +812,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -816,7 +852,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -922,7 +958,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1064,7 +1100,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1072,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A51978F-7647-614D-922C-AF7479B592B3}">
-  <dimension ref="A1:BY104"/>
+  <dimension ref="A1:CK104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB7" workbookViewId="0">
-      <selection activeCell="AO13" sqref="AO13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1094,43 +1130,45 @@
     <col min="14" max="14" width="15" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.83203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="12.5" style="1" customWidth="1"/>
-    <col min="17" max="21" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="10.83203125" style="1"/>
-    <col min="24" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.1640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.1640625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="17.83203125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="18" style="1" customWidth="1"/>
-    <col min="33" max="33" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="24" style="1" customWidth="1"/>
-    <col min="35" max="35" width="27" style="1" customWidth="1"/>
+    <col min="17" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="30" width="11" style="1" customWidth="1"/>
+    <col min="31" max="33" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="10.83203125" style="1"/>
     <col min="36" max="37" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.83203125" style="1"/>
-    <col min="39" max="40" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.83203125" style="1"/>
-    <col min="42" max="42" width="15.6640625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.83203125" style="1"/>
-    <col min="45" max="46" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.83203125" style="1"/>
+    <col min="38" max="38" width="14.1640625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.1640625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="17.83203125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="18" style="1" customWidth="1"/>
+    <col min="45" max="45" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="24" style="1" customWidth="1"/>
+    <col min="47" max="47" width="27" style="1" customWidth="1"/>
     <col min="48" max="49" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="10.83203125" style="1"/>
     <col min="51" max="52" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="10.83203125" style="1"/>
-    <col min="54" max="54" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="59" width="10.83203125" style="1"/>
-    <col min="60" max="60" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="65" width="10.83203125" style="1"/>
-    <col min="66" max="66" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="74" width="10.83203125" style="1"/>
-    <col min="75" max="75" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="16384" width="10.83203125" style="1"/>
+    <col min="54" max="54" width="15.6640625" style="1" customWidth="1"/>
+    <col min="55" max="55" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.83203125" style="1"/>
+    <col min="57" max="58" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.83203125" style="1"/>
+    <col min="60" max="61" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.83203125" style="1"/>
+    <col min="63" max="64" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.83203125" style="1"/>
+    <col min="66" max="66" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="71" width="10.83203125" style="1"/>
+    <col min="72" max="72" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="77" width="10.83203125" style="1"/>
+    <col min="78" max="78" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="79" max="86" width="10.83203125" style="1"/>
+    <col min="87" max="87" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="88" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1186,184 +1224,220 @@
         <v>204</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>92</v>
       </c>
@@ -1419,68 +1493,104 @@
         <v>0</v>
       </c>
       <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
         <v>2</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
+      <c r="AJ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1">
         <v>0.5</v>
       </c>
-      <c r="Z2" s="1">
-        <f>SUM(X2:Y2)/2</f>
+      <c r="AL2" s="1">
+        <f>SUM(AJ2:AK2)/2</f>
         <v>0.25</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="1">
+      <c r="AP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AS2" s="1">
         <v>0.67</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AT2" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="1">
+      <c r="AV2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="1">
         <v>0.1</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM2" s="1">
+      <c r="AY2" s="1">
         <v>0.67</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AZ2" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>93</v>
       </c>
@@ -1533,53 +1643,89 @@
         <v>1773</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1">
         <v>4</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="X3" s="1">
+      <c r="AJ3" s="1">
         <v>0.5</v>
       </c>
-      <c r="Y3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="1">
-        <f t="shared" ref="Z3:Z20" si="0">SUM(X3:Y3)/2</f>
+      <c r="AK3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="1">
+        <f t="shared" ref="AL3:AL20" si="0">SUM(AJ3:AK3)/2</f>
         <v>0.75</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AN3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AO3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD3" s="4">
+      <c r="AP3" s="4">
         <v>9400</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AR3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="1">
+      <c r="AS3" s="1">
         <v>1.2130000000000001</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AU3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ3" s="1">
+      <c r="AV3" s="1">
         <v>-0.03</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AX3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>94</v>
       </c>
@@ -1635,59 +1781,95 @@
         <v>0</v>
       </c>
       <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
         <v>2</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="1">
+      <c r="AJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AO4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="1">
+      <c r="AP4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AR4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AS4" s="1">
         <v>1.87</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AT4" s="1">
         <v>0.02</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AU4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="1">
+      <c r="AV4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="1">
         <v>0.1</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AX4" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
@@ -1743,59 +1925,95 @@
         <v>0</v>
       </c>
       <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
         <v>2</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="AH5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="AI5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="1">
+      <c r="AJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AN5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AO5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD5">
+      <c r="AP5">
         <v>2.27</v>
       </c>
-      <c r="AE5">
+      <c r="AQ5">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AR5" t="s">
         <v>36</v>
       </c>
-      <c r="AG5">
+      <c r="AS5">
         <v>-7.0999999999999994E-2</v>
       </c>
-      <c r="AH5">
+      <c r="AT5">
         <v>1E-3</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AU5" t="s">
         <v>36</v>
       </c>
-      <c r="AJ5">
+      <c r="AV5">
         <v>-6475</v>
       </c>
-      <c r="AK5">
+      <c r="AW5">
         <v>48</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AX5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
@@ -1851,68 +2069,104 @@
         <v>0</v>
       </c>
       <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
         <v>2</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="AH6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="AI6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X6" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="1">
+      <c r="AJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AN6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AO6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="1">
+      <c r="AP6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AR6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG6" s="1">
+      <c r="AS6" s="1">
         <v>0.7</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AT6" s="1">
         <v>0.04</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AU6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK6" s="1">
+      <c r="AV6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW6" s="1">
         <v>0.1</v>
       </c>
-      <c r="AL6" s="1" t="s">
+      <c r="AX6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AM6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="1">
+      <c r="AY6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ6" s="1">
         <v>0.1</v>
       </c>
-      <c r="AO6" s="1" t="s">
+      <c r="BA6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -1968,59 +2222,95 @@
         <v>0</v>
       </c>
       <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
         <v>2</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="AH7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="AI7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="1">
+      <c r="AJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AN7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC7" s="2" t="s">
+      <c r="AO7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="1">
+      <c r="AP7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AR7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AG7" s="1">
+      <c r="AS7" s="1">
         <v>2.1539999999999999</v>
       </c>
-      <c r="AH7" s="1">
+      <c r="AT7" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AU7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ7" s="1">
+      <c r="AV7" s="1">
         <v>-0.17760000000000001</v>
       </c>
-      <c r="AK7" s="1">
+      <c r="AW7" s="1">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AX7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -2076,50 +2366,86 @@
         <v>0</v>
       </c>
       <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
         <v>2</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="AH8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="AI8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X8" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="1">
+      <c r="AJ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AN8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AO8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="1">
+      <c r="AP8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AR8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AS8" s="1">
         <v>2.0179999999999998</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AT8" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="AI8" s="1" t="s">
+      <c r="AU8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>99</v>
       </c>
@@ -2175,77 +2501,113 @@
         <v>0</v>
       </c>
       <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="1">
         <v>2</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="AH9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="AI9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X9" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="1">
+      <c r="AJ9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AN9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AO9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="1">
+      <c r="AP9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ9" s="1">
         <v>0.1</v>
-      </c>
-      <c r="AF9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG9" s="3">
-        <v>2.198</v>
-      </c>
-      <c r="AH9" s="1">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="AI9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ9" s="1">
-        <v>-0.14560000000000001</v>
-      </c>
-      <c r="AK9" s="1">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="AL9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM9" s="1">
-        <v>-0.17760000000000001</v>
-      </c>
-      <c r="AN9" s="1">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="AO9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP9" s="1">
-        <v>-0.17760000000000001</v>
-      </c>
-      <c r="AQ9" s="1">
-        <v>6.4999999999999997E-3</v>
       </c>
       <c r="AR9" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS9" s="3">
+        <v>2.198</v>
+      </c>
+      <c r="AT9" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV9" s="1">
+        <v>-0.14560000000000001</v>
+      </c>
+      <c r="AW9" s="1">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY9" s="1">
+        <v>-0.17760000000000001</v>
+      </c>
+      <c r="AZ9" s="1">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB9" s="1">
+        <v>-0.17760000000000001</v>
+      </c>
+      <c r="BC9" s="1">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="BD9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>100</v>
       </c>
@@ -2301,68 +2663,104 @@
         <v>0</v>
       </c>
       <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="1">
         <v>2</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="AH10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="AI10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X10" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="1">
+      <c r="AJ10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AN10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC10" s="2" t="s">
+      <c r="AO10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD10" s="13">
+      <c r="AP10" s="13">
         <v>5.2</v>
       </c>
-      <c r="AE10" s="1">
+      <c r="AQ10" s="1">
         <v>0.4</v>
       </c>
-      <c r="AF10" s="1" t="s">
+      <c r="AR10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG10" s="1">
+      <c r="AS10" s="1">
         <v>0.67</v>
       </c>
-      <c r="AH10" s="1">
+      <c r="AT10" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI10" s="1" t="s">
+      <c r="AU10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ10" s="1">
+      <c r="AV10" s="1">
         <v>1.897</v>
       </c>
-      <c r="AK10" s="1">
+      <c r="AW10" s="1">
         <v>9.3299999999999994E-2</v>
       </c>
-      <c r="AL10" s="1" t="s">
+      <c r="AX10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM10" s="5">
+      <c r="AY10" s="5">
         <v>79000</v>
       </c>
-      <c r="AN10" s="1">
+      <c r="AZ10" s="1">
         <v>3</v>
       </c>
-      <c r="AO10" s="1" t="s">
+      <c r="BA10" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>104</v>
       </c>
@@ -2418,101 +2816,137 @@
         <v>0</v>
       </c>
       <c r="T11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="1">
         <v>2</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="AH11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="AI11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X11" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="1">
+      <c r="AJ11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL11" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AN11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AO11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD11" s="13">
+      <c r="AP11" s="13">
         <v>1483</v>
       </c>
-      <c r="AE11" s="1">
+      <c r="AQ11" s="1">
         <v>260</v>
       </c>
-      <c r="AF11" s="1" t="s">
+      <c r="AR11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AG11" s="5">
+      <c r="AS11" s="5">
         <v>1E-4</v>
       </c>
-      <c r="AH11" s="1">
+      <c r="AT11" s="1">
         <v>0.03</v>
-      </c>
-      <c r="AI11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ11" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="AK11" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="AL11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM11" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AN11" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AO11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP11" s="1">
-        <v>1.05</v>
-      </c>
-      <c r="AQ11" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="AR11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AS11" s="1">
-        <v>-0.71</v>
-      </c>
-      <c r="AT11" s="1">
-        <v>0.05</v>
       </c>
       <c r="AU11" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AV11" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="AW11" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AX11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY11" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AZ11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="BA11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB11" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="BC11" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="BD11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BE11" s="1">
+        <v>-0.71</v>
+      </c>
+      <c r="BF11" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="BG11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH11" s="1">
         <v>-0.38</v>
       </c>
-      <c r="AW11" s="1">
+      <c r="BI11" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AX11" s="1" t="s">
+      <c r="BJ11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AY11" s="1">
+      <c r="BK11" s="1">
         <v>0.33333299999999999</v>
       </c>
-      <c r="BA11" s="1" t="s">
+      <c r="BM11" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>105</v>
       </c>
@@ -2568,50 +3002,86 @@
         <v>0</v>
       </c>
       <c r="T12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="1">
         <v>2</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="AH12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="AI12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X12" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="1">
+      <c r="AJ12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB12" s="1" t="s">
+      <c r="AN12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC12" s="2" t="s">
+      <c r="AO12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD12" s="4">
+      <c r="AP12" s="4">
         <v>0.44106000000000001</v>
       </c>
-      <c r="AE12" s="1">
+      <c r="AQ12" s="1">
         <v>0.33</v>
       </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AR12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG12" s="1">
+      <c r="AS12" s="1">
         <v>0.77729999999999999</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AT12" s="1">
         <v>6.2190000000000002E-2</v>
       </c>
-      <c r="AI12" s="1" t="s">
+      <c r="AU12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>106</v>
       </c>
@@ -2667,53 +3137,89 @@
         <v>0</v>
       </c>
       <c r="T13" s="1">
+        <v>0</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0</v>
+      </c>
+      <c r="X13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="1">
         <v>2</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="AH13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="AI13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="1">
+      <c r="AJ13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB13" s="1" t="s">
+      <c r="AN13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC13" s="2" t="s">
+      <c r="AO13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD13" s="1">
+      <c r="AP13" s="1">
         <v>5</v>
       </c>
-      <c r="AE13" s="1">
+      <c r="AQ13" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF13" s="1" t="s">
+      <c r="AR13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG13" s="1">
+      <c r="AS13" s="1">
         <v>1.524</v>
       </c>
-      <c r="AI13" s="1" t="s">
+      <c r="AU13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ13" s="1">
+      <c r="AV13" s="1">
         <v>2.6</v>
       </c>
-      <c r="AL13" s="1" t="s">
+      <c r="AX13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
@@ -2769,59 +3275,95 @@
         <v>0</v>
       </c>
       <c r="T14" s="1">
+        <v>0</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0</v>
+      </c>
+      <c r="X14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="1">
         <v>2</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="AH14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="AI14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="1">
+      <c r="AJ14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL14" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AN14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC14" s="2" t="s">
+      <c r="AO14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD14" s="1">
+      <c r="AP14" s="1">
         <v>5</v>
       </c>
-      <c r="AE14" s="1">
+      <c r="AQ14" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF14" s="1" t="s">
+      <c r="AR14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG14" s="1">
+      <c r="AS14" s="1">
         <v>1.5960000000000001</v>
       </c>
-      <c r="AI14" s="1" t="s">
+      <c r="AU14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ14" s="1">
+      <c r="AV14" s="1">
         <v>3.1</v>
       </c>
-      <c r="AL14" s="1" t="s">
+      <c r="AX14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM14" s="1">
+      <c r="AY14" s="1">
         <v>3.1</v>
       </c>
-      <c r="AO14" s="1" t="s">
+      <c r="BA14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>108</v>
       </c>
@@ -2877,140 +3419,176 @@
         <v>0</v>
       </c>
       <c r="T15" s="1">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0</v>
+      </c>
+      <c r="X15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="1">
         <v>2</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="AH15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W15" s="1" t="s">
+      <c r="AI15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="1">
+      <c r="AJ15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB15" s="1" t="s">
+      <c r="AN15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AO15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD15" s="1">
+      <c r="AP15" s="1">
         <v>5</v>
       </c>
-      <c r="AE15" s="1">
+      <c r="AQ15" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF15" s="1" t="s">
+      <c r="AR15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG15" s="1">
+      <c r="AS15" s="1">
         <v>1.327</v>
       </c>
-      <c r="AI15" s="1" t="s">
+      <c r="AU15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ15" s="1">
+      <c r="AV15" s="1">
         <v>2.9</v>
       </c>
-      <c r="AL15" s="1" t="s">
+      <c r="AX15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM15" s="1">
+      <c r="AY15" s="1">
         <v>0.62</v>
       </c>
-      <c r="AO15" s="1" t="s">
+      <c r="BA15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AP15" s="1">
+      <c r="BB15" s="1">
         <v>0.72550000000000003</v>
       </c>
-      <c r="AR15" s="1" t="s">
+      <c r="BD15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AS15" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT15" s="1">
+      <c r="BE15" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF15" s="1">
         <v>0.1</v>
       </c>
-      <c r="AU15" s="1" t="s">
+      <c r="BG15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AV15" s="1">
+      <c r="BH15" s="1">
         <v>1.327</v>
       </c>
-      <c r="AX15" s="1" t="s">
+      <c r="BJ15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AY15" s="1">
+      <c r="BK15" s="1">
         <v>2.9</v>
       </c>
-      <c r="BA15" s="1" t="s">
+      <c r="BM15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="BB15" s="1">
+      <c r="BN15" s="1">
         <v>0.62</v>
       </c>
-      <c r="BD15" s="1" t="s">
+      <c r="BP15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="BE15" s="1">
+      <c r="BQ15" s="1">
         <v>0.72550000000000003</v>
       </c>
-      <c r="BG15" s="1" t="s">
+      <c r="BS15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="BH15" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI15" s="1">
+      <c r="BT15" s="1">
+        <v>1</v>
+      </c>
+      <c r="BU15" s="1">
         <v>0.1</v>
       </c>
-      <c r="BJ15" s="1" t="s">
+      <c r="BV15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="BK15" s="1">
+      <c r="BW15" s="1">
         <v>1.327</v>
       </c>
-      <c r="BM15" s="1" t="s">
+      <c r="BY15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="BN15" s="1">
+      <c r="BZ15" s="1">
         <v>2.9</v>
       </c>
-      <c r="BP15" s="1" t="s">
+      <c r="CB15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="BQ15" s="1">
+      <c r="CC15" s="1">
         <v>0.62</v>
       </c>
-      <c r="BS15" s="1" t="s">
+      <c r="CE15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="BT15" s="1">
+      <c r="CF15" s="1">
         <v>0.72550000000000003</v>
       </c>
-      <c r="BV15" s="1" t="s">
+      <c r="CH15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="BW15" s="1">
-        <v>1</v>
-      </c>
-      <c r="BX15" s="1">
+      <c r="CI15" s="1">
+        <v>1</v>
+      </c>
+      <c r="CJ15" s="1">
         <v>0.1</v>
       </c>
-      <c r="BY15" s="1" t="s">
+      <c r="CK15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:77" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>109</v>
       </c>
@@ -3066,41 +3644,77 @@
         <v>0</v>
       </c>
       <c r="T16" s="1">
+        <v>0</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0</v>
+      </c>
+      <c r="W16" s="1">
+        <v>0</v>
+      </c>
+      <c r="X16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="1">
         <v>2</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="AH16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W16" s="1" t="s">
+      <c r="AI16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z16" s="1">
+      <c r="AJ16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL16" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB16" s="1" t="s">
+      <c r="AN16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC16" s="2" t="s">
+      <c r="AO16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD16" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE16" s="1">
+      <c r="AP16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ16" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF16" s="1" t="s">
+      <c r="AR16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>110</v>
       </c>
@@ -3156,59 +3770,95 @@
         <v>0</v>
       </c>
       <c r="T17" s="1">
+        <v>0</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0</v>
+      </c>
+      <c r="W17" s="1">
+        <v>0</v>
+      </c>
+      <c r="X17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="1">
         <v>2</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="AH17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="AI17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X17" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z17" s="1">
+      <c r="AJ17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL17" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB17" s="1" t="s">
+      <c r="AN17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC17" s="2" t="s">
+      <c r="AO17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD17" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE17" s="1">
+      <c r="AP17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ17" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF17" s="1" t="s">
+      <c r="AR17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG17" s="1">
+      <c r="AS17" s="1">
         <v>1.669</v>
       </c>
-      <c r="AH17" s="1">
+      <c r="AT17" s="1">
         <v>6.2199999999999998E-2</v>
       </c>
-      <c r="AI17" s="1" t="s">
+      <c r="AU17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ17" s="1">
+      <c r="AV17" s="1">
         <v>2.4900000000000002</v>
       </c>
-      <c r="AK17" s="1">
+      <c r="AW17" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AL17" s="1" t="s">
+      <c r="AX17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>111</v>
       </c>
@@ -3264,68 +3914,104 @@
         <v>0</v>
       </c>
       <c r="T18" s="1">
+        <v>0</v>
+      </c>
+      <c r="U18" s="1">
+        <v>0</v>
+      </c>
+      <c r="V18" s="1">
+        <v>0</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0</v>
+      </c>
+      <c r="X18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="1">
         <v>2</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="AH18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="AI18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X18" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="1">
+      <c r="AJ18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB18" s="1" t="s">
+      <c r="AN18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC18" s="2" t="s">
+      <c r="AO18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE18" s="1">
+      <c r="AP18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ18" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF18" s="1" t="s">
+      <c r="AR18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG18" s="1">
+      <c r="AS18" s="1">
         <v>0.91720000000000002</v>
       </c>
-      <c r="AH18" s="1">
+      <c r="AT18" s="1">
         <v>1.0359999999999999E-2</v>
       </c>
-      <c r="AI18" s="1" t="s">
+      <c r="AU18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK18" s="1">
+      <c r="AV18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW18" s="1">
         <v>0.1</v>
       </c>
-      <c r="AL18" s="1" t="s">
+      <c r="AX18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM18" s="1">
+      <c r="AY18" s="1">
         <v>0.91720000000000002</v>
       </c>
-      <c r="AN18" s="1">
+      <c r="AZ18" s="1">
         <v>1.0359999999999999E-2</v>
       </c>
-      <c r="AO18" s="1" t="s">
+      <c r="BA18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
@@ -3381,68 +4067,104 @@
         <v>0</v>
       </c>
       <c r="T19" s="1">
+        <v>0</v>
+      </c>
+      <c r="U19" s="1">
+        <v>0</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0</v>
+      </c>
+      <c r="X19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="1">
         <v>2</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="AH19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W19" s="1" t="s">
+      <c r="AI19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X19" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="1">
+      <c r="AJ19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL19" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB19" s="1" t="s">
+      <c r="AN19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC19" s="2" t="s">
+      <c r="AO19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD19" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="1">
+      <c r="AP19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ19" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF19" s="1" t="s">
+      <c r="AR19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG19" s="1">
+      <c r="AS19" s="1">
         <v>1.03</v>
       </c>
-      <c r="AH19" s="1">
+      <c r="AT19" s="1">
         <v>0.06</v>
       </c>
-      <c r="AI19" s="1" t="s">
+      <c r="AU19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ19" s="1">
+      <c r="AV19" s="1">
         <v>0.74619999999999997</v>
       </c>
-      <c r="AK19" s="1">
+      <c r="AW19" s="1">
         <v>1.55E-2</v>
       </c>
-      <c r="AL19" s="1" t="s">
+      <c r="AX19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM19" s="1">
+      <c r="AY19" s="1">
         <v>0.74619999999999997</v>
       </c>
-      <c r="AN19" s="1">
+      <c r="AZ19" s="1">
         <v>1.55E-2</v>
       </c>
-      <c r="AO19" s="1" t="s">
+      <c r="BA19" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>113</v>
       </c>
@@ -3498,65 +4220,101 @@
         <v>0</v>
       </c>
       <c r="T20" s="1">
+        <v>0</v>
+      </c>
+      <c r="U20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0</v>
+      </c>
+      <c r="W20" s="1">
+        <v>0</v>
+      </c>
+      <c r="X20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="1">
         <v>2</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="AH20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="AI20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X20" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z20" s="1">
+      <c r="AJ20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AN20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC20" s="2" t="s">
+      <c r="AO20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD20" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE20" s="1">
+      <c r="AP20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ20" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF20" s="1" t="s">
+      <c r="AR20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG20" s="1">
+      <c r="AS20" s="1">
         <v>1.88</v>
       </c>
-      <c r="AH20" s="1">
+      <c r="AT20" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI20" s="1" t="s">
+      <c r="AU20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ20" s="1">
+      <c r="AV20" s="1">
         <v>2.58</v>
       </c>
-      <c r="AK20" s="1">
+      <c r="AW20" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AL20" s="1" t="s">
+      <c r="AX20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM20" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO20" s="1" t="s">
+      <c r="AY20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>113</v>
       </c>
@@ -3612,65 +4370,101 @@
         <v>0</v>
       </c>
       <c r="T21" s="1">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
+      <c r="W21" s="1">
+        <v>0</v>
+      </c>
+      <c r="X21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="1">
         <v>2</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="AH21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W21" s="1" t="s">
+      <c r="AI21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X21" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z21" s="1">
-        <f t="shared" ref="Z21:Z23" si="1">SUM(X21:Y21)/2</f>
+      <c r="AJ21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL21" s="1">
+        <f t="shared" ref="AL21:AL23" si="1">SUM(AJ21:AK21)/2</f>
         <v>0.5</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AN21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC21" s="2" t="s">
+      <c r="AO21" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="AD21" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="1">
+      <c r="AP21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ21" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF21" s="1" t="s">
+      <c r="AR21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG21" s="1">
+      <c r="AS21" s="1">
         <v>1.88</v>
       </c>
-      <c r="AH21" s="1">
+      <c r="AT21" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI21" s="1" t="s">
+      <c r="AU21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ21" s="1">
+      <c r="AV21" s="1">
         <v>2.58</v>
       </c>
-      <c r="AK21" s="1">
+      <c r="AW21" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AL21" s="1" t="s">
+      <c r="AX21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM21" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO21" s="1" t="s">
+      <c r="AY21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA21" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>113</v>
       </c>
@@ -3726,65 +4520,101 @@
         <v>0</v>
       </c>
       <c r="T22" s="1">
+        <v>0</v>
+      </c>
+      <c r="U22" s="1">
+        <v>0</v>
+      </c>
+      <c r="V22" s="1">
+        <v>0</v>
+      </c>
+      <c r="W22" s="1">
+        <v>0</v>
+      </c>
+      <c r="X22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="1">
         <v>2</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="AH22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W22" s="1" t="s">
+      <c r="AI22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X22" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z22" s="1">
+      <c r="AJ22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL22" s="1">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AN22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC22" s="2" t="s">
+      <c r="AO22" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AD22" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE22" s="1">
+      <c r="AP22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ22" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF22" s="1" t="s">
+      <c r="AR22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG22" s="1">
+      <c r="AS22" s="1">
         <v>1.88</v>
       </c>
-      <c r="AH22" s="1">
+      <c r="AT22" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI22" s="1" t="s">
+      <c r="AU22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ22" s="1">
+      <c r="AV22" s="1">
         <v>2.58</v>
       </c>
-      <c r="AK22" s="1">
+      <c r="AW22" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AL22" s="1" t="s">
+      <c r="AX22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM22" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO22" s="1" t="s">
+      <c r="AY22" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>113</v>
       </c>
@@ -3840,65 +4670,101 @@
         <v>0</v>
       </c>
       <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>0</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
+      <c r="W23" s="1">
+        <v>0</v>
+      </c>
+      <c r="X23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="1">
         <v>2</v>
       </c>
-      <c r="V23" s="1" t="s">
+      <c r="AH23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W23" s="1" t="s">
+      <c r="AI23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X23" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z23" s="1">
+      <c r="AJ23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="1">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="AB23" s="1" t="s">
+      <c r="AN23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC23" s="2" t="s">
+      <c r="AO23" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AD23" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE23" s="1">
+      <c r="AP23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ23" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF23" s="1" t="s">
+      <c r="AR23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG23" s="1">
+      <c r="AS23" s="1">
         <v>1.88</v>
       </c>
-      <c r="AH23" s="1">
+      <c r="AT23" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI23" s="1" t="s">
+      <c r="AU23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ23" s="1">
+      <c r="AV23" s="1">
         <v>2.58</v>
       </c>
-      <c r="AK23" s="1">
+      <c r="AW23" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AL23" s="1" t="s">
+      <c r="AX23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM23" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO23" s="1" t="s">
+      <c r="AY23" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA23" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>185</v>
       </c>
@@ -3954,71 +4820,107 @@
         <v>0</v>
       </c>
       <c r="T24" s="1">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1">
+        <v>0</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0</v>
+      </c>
+      <c r="W24" s="1">
+        <v>0</v>
+      </c>
+      <c r="X24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="1">
         <v>2</v>
       </c>
-      <c r="V24" s="1" t="s">
+      <c r="AH24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W24" s="1" t="s">
+      <c r="AI24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X24" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z24" s="1">
-        <f t="shared" ref="Z24:Z26" si="2">SUM(X24:Y24)/2</f>
+      <c r="AJ24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL24" s="1">
+        <f t="shared" ref="AL24:AL26" si="2">SUM(AJ24:AK24)/2</f>
         <v>0.5</v>
       </c>
-      <c r="AB24" s="1" t="s">
+      <c r="AN24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC24" s="2" t="s">
+      <c r="AO24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD24" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE24" s="1">
+      <c r="AP24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ24" s="1">
         <v>0.1</v>
       </c>
-      <c r="AF24" s="1" t="s">
+      <c r="AR24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG24" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH24" s="1">
+      <c r="AS24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT24" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI24" s="1" t="s">
+      <c r="AU24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ24" s="1">
+      <c r="AV24" s="1">
         <v>-0.01</v>
       </c>
-      <c r="AK24" s="1">
+      <c r="AW24" s="1">
         <v>1E-3</v>
       </c>
-      <c r="AL24" s="1" t="s">
+      <c r="AX24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AM24" s="4">
+      <c r="AY24" s="4">
         <v>0.5</v>
       </c>
-      <c r="AO24" s="1" t="s">
+      <c r="BA24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AP24" s="1">
+      <c r="BB24" s="1">
         <v>1000</v>
       </c>
-      <c r="AR24" s="1" t="s">
+      <c r="BD24" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>186</v>
       </c>
@@ -4074,68 +4976,104 @@
         <v>0</v>
       </c>
       <c r="T25" s="1">
+        <v>0</v>
+      </c>
+      <c r="U25" s="1">
+        <v>0</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0</v>
+      </c>
+      <c r="W25" s="1">
+        <v>0</v>
+      </c>
+      <c r="X25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="1">
         <v>2</v>
       </c>
-      <c r="V25" s="1" t="s">
+      <c r="AH25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W25" s="1" t="s">
+      <c r="AI25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="1">
+      <c r="AJ25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL25" s="1">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="AB25" s="1" t="s">
+      <c r="AN25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC25" s="2" t="s">
+      <c r="AO25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE25" s="1">
+      <c r="AP25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ25" s="1">
         <v>0.1</v>
-      </c>
-      <c r="AF25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG25" s="1">
-        <v>-5</v>
-      </c>
-      <c r="AI25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK25" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AL25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP25" s="1">
-        <v>300</v>
       </c>
       <c r="AR25" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS25" s="1">
+        <v>-5</v>
+      </c>
+      <c r="AU25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW25" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AX25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY25" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB25" s="1">
+        <v>300</v>
+      </c>
+      <c r="BD25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>187</v>
       </c>
@@ -4191,68 +5129,104 @@
         <v>0</v>
       </c>
       <c r="T26" s="1">
+        <v>0</v>
+      </c>
+      <c r="U26" s="1">
+        <v>0</v>
+      </c>
+      <c r="V26" s="1">
+        <v>0</v>
+      </c>
+      <c r="W26" s="1">
+        <v>0</v>
+      </c>
+      <c r="X26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="1">
         <v>2</v>
       </c>
-      <c r="V26" s="1" t="s">
+      <c r="AH26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W26" s="1" t="s">
+      <c r="AI26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X26" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z26" s="1">
+      <c r="AJ26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL26" s="1">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="AB26" s="1" t="s">
+      <c r="AN26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC26" s="2" t="s">
+      <c r="AO26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD26" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE26" s="1">
+      <c r="AP26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ26" s="1">
         <v>0.1</v>
-      </c>
-      <c r="AF26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG26" s="1">
-        <v>-5</v>
-      </c>
-      <c r="AI26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ26" s="1">
-        <v>1</v>
-      </c>
-      <c r="AK26" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AL26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM26" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP26" s="1">
-        <v>300</v>
       </c>
       <c r="AR26" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AS26" s="1">
+        <v>-5</v>
+      </c>
+      <c r="AU26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AX26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY26" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB26" s="1">
+        <v>300</v>
+      </c>
+      <c r="BD26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>105</v>
       </c>
@@ -4308,50 +5282,86 @@
         <v>0</v>
       </c>
       <c r="T27" s="1">
+        <v>0</v>
+      </c>
+      <c r="U27" s="1">
+        <v>0</v>
+      </c>
+      <c r="V27" s="1">
+        <v>0</v>
+      </c>
+      <c r="W27" s="1">
+        <v>0</v>
+      </c>
+      <c r="X27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="1">
         <v>2</v>
       </c>
-      <c r="V27" s="1" t="s">
+      <c r="AH27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W27" s="1" t="s">
+      <c r="AI27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X27" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z27" s="1">
-        <f t="shared" ref="Z27:Z29" si="3">SUM(X27:Y27)/2</f>
+      <c r="AJ27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL27" s="1">
+        <f t="shared" ref="AL27:AL29" si="3">SUM(AJ27:AK27)/2</f>
         <v>0.5</v>
       </c>
-      <c r="AB27" s="1" t="s">
+      <c r="AN27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC27" s="2" t="s">
+      <c r="AO27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD27" s="4">
+      <c r="AP27" s="4">
         <v>5.0199999999999996</v>
       </c>
-      <c r="AE27" s="1">
+      <c r="AQ27" s="1">
         <v>0.48</v>
       </c>
-      <c r="AF27" s="1" t="s">
+      <c r="AR27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG27" s="1">
+      <c r="AS27" s="1">
         <v>1.2989999999999999</v>
       </c>
-      <c r="AH27" s="1">
+      <c r="AT27" s="1">
         <v>0.114</v>
       </c>
-      <c r="AI27" s="1" t="s">
+      <c r="AU27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>105</v>
       </c>
@@ -4407,50 +5417,86 @@
         <v>0</v>
       </c>
       <c r="T28" s="1">
+        <v>0</v>
+      </c>
+      <c r="U28" s="1">
+        <v>0</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0</v>
+      </c>
+      <c r="X28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="1">
         <v>2</v>
       </c>
-      <c r="V28" s="1" t="s">
+      <c r="AH28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="AI28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X28" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z28" s="1">
+      <c r="AJ28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL28" s="1">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="AB28" s="1" t="s">
+      <c r="AN28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC28" s="2" t="s">
+      <c r="AO28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD28" s="4">
+      <c r="AP28" s="4">
         <v>5.0199999999999996</v>
       </c>
-      <c r="AE28" s="1">
+      <c r="AQ28" s="1">
         <v>0.48</v>
       </c>
-      <c r="AF28" s="1" t="s">
+      <c r="AR28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG28" s="1">
+      <c r="AS28" s="1">
         <v>1.399</v>
       </c>
-      <c r="AH28" s="1">
+      <c r="AT28" s="1">
         <v>0.114</v>
       </c>
-      <c r="AI28" s="1" t="s">
+      <c r="AU28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>105</v>
       </c>
@@ -4506,46 +5552,82 @@
         <v>0</v>
       </c>
       <c r="T29" s="1">
+        <v>0</v>
+      </c>
+      <c r="U29" s="1">
+        <v>0</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0</v>
+      </c>
+      <c r="W29" s="1">
+        <v>0</v>
+      </c>
+      <c r="X29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="1">
         <v>2</v>
       </c>
-      <c r="V29" s="1" t="s">
+      <c r="AH29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W29" s="1" t="s">
+      <c r="AI29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X29" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z29" s="1">
+      <c r="AJ29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL29" s="1">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="AB29" s="1" t="s">
+      <c r="AN29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AC29" s="2" t="s">
+      <c r="AO29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD29" s="4">
+      <c r="AP29" s="4">
         <v>4.0199999999999996</v>
       </c>
-      <c r="AE29" s="1">
+      <c r="AQ29" s="1">
         <v>0.48</v>
       </c>
-      <c r="AF29" s="1" t="s">
+      <c r="AR29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG29" s="1">
+      <c r="AS29" s="1">
         <v>1.1990000000000001</v>
       </c>
-      <c r="AH29" s="1">
+      <c r="AT29" s="1">
         <v>0.114</v>
       </c>
-      <c r="AI29" s="1" t="s">
+      <c r="AU29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4567,185 +5649,197 @@
     <row r="42" spans="2:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="7"/>
     </row>
-    <row r="51" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AD51" s="3"/>
-    </row>
-    <row r="61" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:42" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP51" s="3"/>
+    </row>
+    <row r="61" spans="1:42" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:42" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:42" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:42" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG66" s="4"/>
-    </row>
-    <row r="67" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG67" s="4"/>
-    </row>
-    <row r="68" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG68" s="4"/>
-    </row>
-    <row r="69" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AD69" s="5"/>
-      <c r="AJ69" s="5"/>
-      <c r="AS69" s="5"/>
-      <c r="AY69" s="5"/>
-      <c r="BB69" s="5"/>
-      <c r="BH69" s="5"/>
-      <c r="BW69" s="5"/>
-    </row>
-    <row r="70" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS66" s="4"/>
+    </row>
+    <row r="67" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS67" s="4"/>
+    </row>
+    <row r="68" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS68" s="4"/>
+    </row>
+    <row r="69" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP69" s="5"/>
+      <c r="AV69" s="5"/>
+      <c r="BE69" s="5"/>
+      <c r="BK69" s="5"/>
+      <c r="BN69" s="5"/>
+      <c r="BT69" s="5"/>
+      <c r="CI69" s="5"/>
+    </row>
+    <row r="70" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D70" s="9"/>
       <c r="N70"/>
-      <c r="T70"/>
-      <c r="AB70"/>
-    </row>
-    <row r="71" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF70"/>
+      <c r="AN70"/>
+    </row>
+    <row r="71" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D71" s="9"/>
       <c r="N71"/>
       <c r="Q71"/>
       <c r="R71"/>
+      <c r="S71"/>
       <c r="T71"/>
-    </row>
-    <row r="72" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U71"/>
+      <c r="V71"/>
+      <c r="W71"/>
+      <c r="X71"/>
+      <c r="Y71"/>
+      <c r="Z71"/>
+      <c r="AA71"/>
+      <c r="AB71"/>
+      <c r="AC71"/>
+      <c r="AD71"/>
+      <c r="AF71"/>
+    </row>
+    <row r="72" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C76"/>
       <c r="D76" s="8"/>
       <c r="Q76"/>
-      <c r="T76"/>
-      <c r="AD76" s="5"/>
-      <c r="AE76" s="5"/>
-      <c r="AM76" s="5"/>
-      <c r="AN76" s="5"/>
-    </row>
-    <row r="77" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AF76"/>
+      <c r="AP76" s="5"/>
+      <c r="AQ76" s="5"/>
+      <c r="AY76" s="5"/>
+      <c r="AZ76" s="5"/>
+    </row>
+    <row r="77" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C77"/>
       <c r="D77" s="8"/>
       <c r="Q77"/>
-      <c r="AD77" s="5"/>
-      <c r="AE77" s="5"/>
-      <c r="AM77" s="5"/>
-      <c r="AN77" s="5"/>
-    </row>
-    <row r="78" spans="1:75" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP77" s="5"/>
+      <c r="AQ77" s="5"/>
+      <c r="AY77" s="5"/>
+      <c r="AZ77" s="5"/>
+    </row>
+    <row r="78" spans="1:87" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78"/>
       <c r="D78" s="8"/>
       <c r="Q78"/>
-      <c r="AD78" s="5"/>
-      <c r="AE78" s="5"/>
-      <c r="AM78" s="5"/>
-      <c r="AN78" s="5"/>
-    </row>
-    <row r="82" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP78" s="5"/>
+      <c r="AQ78" s="5"/>
+      <c r="AY78" s="5"/>
+      <c r="AZ78" s="5"/>
+    </row>
+    <row r="82" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D82" s="8"/>
-      <c r="V82"/>
-    </row>
-    <row r="83" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH82"/>
+    </row>
+    <row r="83" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D83" s="8"/>
-      <c r="V83"/>
-    </row>
-    <row r="84" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH83"/>
+    </row>
+    <row r="84" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D84" s="8"/>
-      <c r="V84"/>
-    </row>
-    <row r="85" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH84"/>
+    </row>
+    <row r="85" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D85" s="8"/>
-      <c r="V85"/>
-    </row>
-    <row r="86" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH85"/>
+    </row>
+    <row r="86" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="10"/>
       <c r="D86" s="1"/>
       <c r="J86" s="11"/>
-      <c r="V86"/>
-    </row>
-    <row r="87" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH86"/>
+    </row>
+    <row r="87" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="10"/>
       <c r="D87" s="1"/>
       <c r="J87" s="11"/>
-      <c r="V87"/>
-    </row>
-    <row r="88" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH87"/>
+    </row>
+    <row r="88" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="10"/>
       <c r="D88" s="1"/>
       <c r="J88" s="11"/>
-      <c r="V88"/>
-    </row>
-    <row r="89" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AH88"/>
+    </row>
+    <row r="89" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="10"/>
       <c r="D89" s="1"/>
       <c r="J89" s="11"/>
     </row>
-    <row r="90" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="10"/>
       <c r="D90" s="1"/>
       <c r="J90" s="11"/>
     </row>
-    <row r="91" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="10"/>
       <c r="D91" s="1"/>
       <c r="J91" s="11"/>
     </row>
-    <row r="92" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="10"/>
       <c r="D92" s="1"/>
       <c r="J92" s="11"/>
     </row>
-    <row r="93" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="10"/>
       <c r="D93" s="1"/>
       <c r="J93" s="11"/>
     </row>
-    <row r="94" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="10"/>
       <c r="D94" s="1"/>
       <c r="J94" s="11"/>
     </row>
-    <row r="96" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AJ96" s="2"/>
-    </row>
-    <row r="100" spans="33:34" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG100" s="2"/>
-      <c r="AH100" s="2"/>
-    </row>
-    <row r="101" spans="33:34" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG101" s="2"/>
-      <c r="AH101" s="2"/>
-    </row>
-    <row r="102" spans="33:34" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG102" s="2"/>
-      <c r="AH102" s="2"/>
-    </row>
-    <row r="103" spans="33:34" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG103" s="2"/>
-      <c r="AH103" s="2"/>
-    </row>
-    <row r="104" spans="33:34" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AG104" s="2"/>
-      <c r="AH104" s="2"/>
+    <row r="96" spans="1:48" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AV96" s="2"/>
+    </row>
+    <row r="100" spans="45:46" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS100" s="2"/>
+      <c r="AT100" s="2"/>
+    </row>
+    <row r="101" spans="45:46" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS101" s="2"/>
+      <c r="AT101" s="2"/>
+    </row>
+    <row r="102" spans="45:46" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS102" s="2"/>
+      <c r="AT102" s="2"/>
+    </row>
+    <row r="103" spans="45:46" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS103" s="2"/>
+      <c r="AT103" s="2"/>
+    </row>
+    <row r="104" spans="45:46" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AS104" s="2"/>
+      <c r="AT104" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
major changes to mixing, models, utils, and mechanisms. Biggest change is added documentation to every class and class method. Added unit tests for most mixing models
</commit_message>
<xml_diff>
--- a/test/test_database.xlsx
+++ b/test/test_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/X9 Pro/Recovered Data  - EXFAT/MT_RESEARCH/2D_Petrology/mineral_conductivity/mineralconductivities/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{673E85B5-CA5F-B748-8F67-8DF124AB6D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7772122F-BED3-024D-9227-5A60A52E900D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16680" xr2:uid="{EF1EAB3C-7106-8347-9382-DA47A6680CFD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{EF1EAB3C-7106-8347-9382-DA47A6680CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="test_database" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Eq ID</t>
   </si>
   <si>
-    <t>arrhenious_simple</t>
-  </si>
-  <si>
     <t>Water Min</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Phase Type</t>
   </si>
   <si>
-    <t>arrhenious_log_fO2</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -125,18 +119,12 @@
     <t>wtpct</t>
   </si>
   <si>
-    <t>water_exponent_arrhenious</t>
-  </si>
-  <si>
     <t>Iron units</t>
   </si>
   <si>
     <t xml:space="preserve">Mo–MoO2 </t>
   </si>
   <si>
-    <t>water_exponent_arrhenious_pressure</t>
-  </si>
-  <si>
     <t>preexp_log</t>
   </si>
   <si>
@@ -170,18 +158,9 @@
     <t>h_uncertainty</t>
   </si>
   <si>
-    <t>arrhenious_preexp_parameterized</t>
-  </si>
-  <si>
-    <t>arrhenious_pressure</t>
-  </si>
-  <si>
     <t>single_value</t>
   </si>
   <si>
-    <t>arrhenious_fugacity</t>
-  </si>
-  <si>
     <t>seo3_eq</t>
   </si>
   <si>
@@ -296,18 +275,6 @@
     <t>a_uncertainty</t>
   </si>
   <si>
-    <t>arrhenious_logfO2_2</t>
-  </si>
-  <si>
-    <t>iron_preexp_enthalpy_arrhenious</t>
-  </si>
-  <si>
-    <t>iron_water_arrhenious1</t>
-  </si>
-  <si>
-    <t>iron_water_arrhenious2</t>
-  </si>
-  <si>
     <t>nerst_einstein1</t>
   </si>
   <si>
@@ -347,12 +314,6 @@
     <t>nerst_einstein_2</t>
   </si>
   <si>
-    <t>water_exponent_arrhenious_pressure_invT</t>
-  </si>
-  <si>
-    <t>water_preexp_enthalpy_arrhenious</t>
-  </si>
-  <si>
     <t>Test10</t>
   </si>
   <si>
@@ -593,9 +554,6 @@
     <t>vft_wet</t>
   </si>
   <si>
-    <t>linked_arrhenious_wet</t>
-  </si>
-  <si>
     <t>Test 20</t>
   </si>
   <si>
@@ -656,9 +614,6 @@
     <t>Temp Max</t>
   </si>
   <si>
-    <t>arrhenious_simple+arrhenious_simple</t>
-  </si>
-  <si>
     <t>Na2o Min</t>
   </si>
   <si>
@@ -693,6 +648,51 @@
   </si>
   <si>
     <t>CO2 average</t>
+  </si>
+  <si>
+    <t>arrhenius_simple+arrhenius_simple</t>
+  </si>
+  <si>
+    <t>arrhenius_fugacity</t>
+  </si>
+  <si>
+    <t>arrhenius_log_fO2</t>
+  </si>
+  <si>
+    <t>arrhenius_logfO2_2</t>
+  </si>
+  <si>
+    <t>arrhenius_preexp_parameterized</t>
+  </si>
+  <si>
+    <t>arrhenius_pressure</t>
+  </si>
+  <si>
+    <t>arrhenius_simple</t>
+  </si>
+  <si>
+    <t>iron_preexp_enthalpy_arrhenius</t>
+  </si>
+  <si>
+    <t>iron_water_arrhenius1</t>
+  </si>
+  <si>
+    <t>iron_water_arrhenius2</t>
+  </si>
+  <si>
+    <t>water_exponent_arrhenius</t>
+  </si>
+  <si>
+    <t>water_exponent_arrhenius_pressure</t>
+  </si>
+  <si>
+    <t>water_exponent_arrhenius_pressure_invT</t>
+  </si>
+  <si>
+    <t>water_preexp_enthalpy_arrhenius</t>
+  </si>
+  <si>
+    <t>linked_arrhenius_wet</t>
   </si>
 </sst>
 </file>
@@ -1110,8 +1110,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A51978F-7647-614D-922C-AF7479B592B3}">
   <dimension ref="A1:CK104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:U29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1182,300 +1182,300 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AO1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AQ1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BF1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AU1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BL1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BP1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BH1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BK1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="CH1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="CI1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
@@ -1532,10 +1532,10 @@
         <v>2</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ2" s="1">
         <v>0</v>
@@ -1548,10 +1548,10 @@
         <v>0.25</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP2" s="1">
         <v>1</v>
@@ -1560,7 +1560,7 @@
         <v>0.1</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS2" s="1">
         <v>0.67</v>
@@ -1569,7 +1569,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AV2" s="1">
         <v>1</v>
@@ -1578,7 +1578,7 @@
         <v>0.1</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AY2" s="1">
         <v>0.67</v>
@@ -1587,48 +1587,48 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>204</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O3" s="1">
         <v>2</v>
@@ -1685,10 +1685,10 @@
         <v>4</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="AJ3" s="1">
         <v>0.5</v>
@@ -1701,69 +1701,69 @@
         <v>0.75</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP3" s="4">
         <v>9400</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AS3" s="1">
         <v>1.2130000000000001</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV3" s="1">
         <v>-0.03</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>22</v>
+        <v>205</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O4" s="1">
         <v>1</v>
@@ -1820,10 +1820,10 @@
         <v>2</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ4" s="1">
         <v>0</v>
@@ -1836,10 +1836,10 @@
         <v>0.5</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP4" s="1">
         <v>1</v>
@@ -1848,7 +1848,7 @@
         <v>0.1</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS4" s="1">
         <v>1.87</v>
@@ -1857,7 +1857,7 @@
         <v>0.02</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV4" s="1">
         <v>1</v>
@@ -1866,48 +1866,48 @@
         <v>0.1</v>
       </c>
       <c r="AX4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>85</v>
+        <v>206</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O5" s="1">
         <v>1</v>
@@ -1964,10 +1964,10 @@
         <v>2</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ5" s="1">
         <v>0</v>
@@ -1980,10 +1980,10 @@
         <v>0.5</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP5">
         <v>2.27</v>
@@ -1992,7 +1992,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="AR5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AS5">
         <v>-7.0999999999999994E-2</v>
@@ -2001,7 +2001,7 @@
         <v>1E-3</v>
       </c>
       <c r="AU5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AV5">
         <v>-6475</v>
@@ -2010,48 +2010,48 @@
         <v>48</v>
       </c>
       <c r="AX5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>43</v>
+        <v>207</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O6" s="1">
         <v>1</v>
@@ -2108,10 +2108,10 @@
         <v>2</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ6" s="1">
         <v>0</v>
@@ -2124,10 +2124,10 @@
         <v>0.5</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP6" s="1">
         <v>1</v>
@@ -2136,7 +2136,7 @@
         <v>0.1</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS6" s="1">
         <v>0.7</v>
@@ -2145,7 +2145,7 @@
         <v>0.04</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV6" s="1">
         <v>1</v>
@@ -2154,7 +2154,7 @@
         <v>0.1</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AY6" s="1">
         <v>1</v>
@@ -2163,48 +2163,48 @@
         <v>0.1</v>
       </c>
       <c r="BA6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>44</v>
+        <v>208</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O7" s="1">
         <v>1</v>
@@ -2261,10 +2261,10 @@
         <v>2</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ7" s="1">
         <v>0</v>
@@ -2277,10 +2277,10 @@
         <v>0.5</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP7" s="1">
         <v>1</v>
@@ -2289,7 +2289,7 @@
         <v>0.1</v>
       </c>
       <c r="AR7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AS7" s="1">
         <v>2.1539999999999999</v>
@@ -2298,7 +2298,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="AU7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV7" s="1">
         <v>-0.17760000000000001</v>
@@ -2307,48 +2307,48 @@
         <v>6.4999999999999997E-3</v>
       </c>
       <c r="AX7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>170</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O8" s="1">
         <v>1</v>
@@ -2405,10 +2405,10 @@
         <v>2</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
@@ -2421,10 +2421,10 @@
         <v>0.5</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP8" s="1">
         <v>1</v>
@@ -2433,7 +2433,7 @@
         <v>0.1</v>
       </c>
       <c r="AR8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AS8" s="1">
         <v>2.0179999999999998</v>
@@ -2442,48 +2442,48 @@
         <v>4.7E-2</v>
       </c>
       <c r="AU8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O9" s="1">
         <v>1</v>
@@ -2540,10 +2540,10 @@
         <v>2</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ9" s="1">
         <v>0</v>
@@ -2556,10 +2556,10 @@
         <v>0.5</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP9" s="1">
         <v>1</v>
@@ -2568,7 +2568,7 @@
         <v>0.1</v>
       </c>
       <c r="AR9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AS9" s="3">
         <v>2.198</v>
@@ -2577,7 +2577,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="AU9" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV9" s="1">
         <v>-0.14560000000000001</v>
@@ -2586,7 +2586,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AY9" s="1">
         <v>-0.17760000000000001</v>
@@ -2595,7 +2595,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
       <c r="BA9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="BB9" s="1">
         <v>-0.17760000000000001</v>
@@ -2604,48 +2604,48 @@
         <v>6.4999999999999997E-3</v>
       </c>
       <c r="BD9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O10" s="1">
         <v>1</v>
@@ -2702,10 +2702,10 @@
         <v>2</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ10" s="1">
         <v>0</v>
@@ -2718,10 +2718,10 @@
         <v>0.5</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP10" s="13">
         <v>5.2</v>
@@ -2730,7 +2730,7 @@
         <v>0.4</v>
       </c>
       <c r="AR10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS10" s="1">
         <v>0.67</v>
@@ -2739,7 +2739,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AV10" s="1">
         <v>1.897</v>
@@ -2748,7 +2748,7 @@
         <v>9.3299999999999994E-2</v>
       </c>
       <c r="AX10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AY10" s="5">
         <v>79000</v>
@@ -2757,48 +2757,48 @@
         <v>3</v>
       </c>
       <c r="BA10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C11" s="1">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>88</v>
+        <v>212</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O11" s="1">
         <v>1</v>
@@ -2855,10 +2855,10 @@
         <v>2</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ11" s="1">
         <v>0</v>
@@ -2871,10 +2871,10 @@
         <v>0.5</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP11" s="13">
         <v>1483</v>
@@ -2883,7 +2883,7 @@
         <v>260</v>
       </c>
       <c r="AR11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AS11" s="5">
         <v>1E-4</v>
@@ -2892,7 +2892,7 @@
         <v>0.03</v>
       </c>
       <c r="AU11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AV11" s="1">
         <v>0.09</v>
@@ -2901,7 +2901,7 @@
         <v>0.03</v>
       </c>
       <c r="AX11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AY11" s="1">
         <v>1.1000000000000001</v>
@@ -2910,7 +2910,7 @@
         <v>0.1</v>
       </c>
       <c r="BA11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BB11" s="1">
         <v>1.05</v>
@@ -2919,7 +2919,7 @@
         <v>0.03</v>
       </c>
       <c r="BD11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="BE11" s="1">
         <v>-0.71</v>
@@ -2928,7 +2928,7 @@
         <v>0.05</v>
       </c>
       <c r="BG11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="BH11" s="1">
         <v>-0.38</v>
@@ -2937,54 +2937,54 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="BJ11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="BK11" s="1">
         <v>0.33333299999999999</v>
       </c>
       <c r="BM11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C12" s="1">
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O12" s="1">
         <v>1</v>
@@ -3041,10 +3041,10 @@
         <v>2</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ12" s="1">
         <v>0</v>
@@ -3057,10 +3057,10 @@
         <v>0.5</v>
       </c>
       <c r="AN12" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP12" s="4">
         <v>0.44106000000000001</v>
@@ -3069,7 +3069,7 @@
         <v>0.33</v>
       </c>
       <c r="AR12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS12" s="1">
         <v>0.77729999999999999</v>
@@ -3078,48 +3078,48 @@
         <v>6.2190000000000002E-2</v>
       </c>
       <c r="AU12" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C13" s="1">
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O13" s="1">
         <v>1</v>
@@ -3176,10 +3176,10 @@
         <v>2</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ13" s="1">
         <v>0</v>
@@ -3192,10 +3192,10 @@
         <v>0.5</v>
       </c>
       <c r="AN13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP13" s="1">
         <v>5</v>
@@ -3204,60 +3204,60 @@
         <v>0.1</v>
       </c>
       <c r="AR13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS13" s="1">
         <v>1.524</v>
       </c>
       <c r="AU13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV13" s="1">
         <v>2.6</v>
       </c>
       <c r="AX13" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C14" s="1">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O14" s="1">
         <v>1</v>
@@ -3314,10 +3314,10 @@
         <v>2</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ14" s="1">
         <v>0</v>
@@ -3330,10 +3330,10 @@
         <v>0.5</v>
       </c>
       <c r="AN14" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP14" s="1">
         <v>5</v>
@@ -3342,66 +3342,66 @@
         <v>0.1</v>
       </c>
       <c r="AR14" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS14" s="1">
         <v>1.5960000000000001</v>
       </c>
       <c r="AU14" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV14" s="1">
         <v>3.1</v>
       </c>
       <c r="AX14" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AY14" s="1">
         <v>3.1</v>
       </c>
       <c r="BA14" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C15" s="1">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O15" s="1">
         <v>1</v>
@@ -3458,10 +3458,10 @@
         <v>2</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ15" s="1">
         <v>0</v>
@@ -3474,10 +3474,10 @@
         <v>0.5</v>
       </c>
       <c r="AN15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP15" s="1">
         <v>5</v>
@@ -3486,31 +3486,31 @@
         <v>0.1</v>
       </c>
       <c r="AR15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS15" s="1">
         <v>1.327</v>
       </c>
       <c r="AU15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV15" s="1">
         <v>2.9</v>
       </c>
       <c r="AX15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AY15" s="1">
         <v>0.62</v>
       </c>
       <c r="BA15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BB15" s="1">
         <v>0.72550000000000003</v>
       </c>
       <c r="BD15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="BE15" s="1">
         <v>1</v>
@@ -3519,31 +3519,31 @@
         <v>0.1</v>
       </c>
       <c r="BG15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="BH15" s="1">
         <v>1.327</v>
       </c>
       <c r="BJ15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="BK15" s="1">
         <v>2.9</v>
       </c>
       <c r="BM15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="BN15" s="1">
         <v>0.62</v>
       </c>
       <c r="BP15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BQ15" s="1">
         <v>0.72550000000000003</v>
       </c>
       <c r="BS15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="BT15" s="1">
         <v>1</v>
@@ -3552,31 +3552,31 @@
         <v>0.1</v>
       </c>
       <c r="BV15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="BW15" s="1">
         <v>1.327</v>
       </c>
       <c r="BY15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="BZ15" s="1">
         <v>2.9</v>
       </c>
       <c r="CB15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="CC15" s="1">
         <v>0.62</v>
       </c>
       <c r="CE15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="CF15" s="1">
         <v>0.72550000000000003</v>
       </c>
       <c r="CH15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="CI15" s="1">
         <v>1</v>
@@ -3585,48 +3585,48 @@
         <v>0.1</v>
       </c>
       <c r="CK15" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:89" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C16" s="1">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O16" s="1">
         <v>1</v>
@@ -3683,10 +3683,10 @@
         <v>2</v>
       </c>
       <c r="AH16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ16" s="1">
         <v>0</v>
@@ -3699,10 +3699,10 @@
         <v>0.5</v>
       </c>
       <c r="AN16" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP16" s="1">
         <v>1</v>
@@ -3711,48 +3711,48 @@
         <v>0.1</v>
       </c>
       <c r="AR16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C17" s="1">
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>28</v>
+        <v>213</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O17" s="1">
         <v>1</v>
@@ -3809,10 +3809,10 @@
         <v>2</v>
       </c>
       <c r="AH17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ17" s="1">
         <v>0</v>
@@ -3825,10 +3825,10 @@
         <v>0.5</v>
       </c>
       <c r="AN17" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP17" s="1">
         <v>1</v>
@@ -3837,7 +3837,7 @@
         <v>0.1</v>
       </c>
       <c r="AR17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS17" s="1">
         <v>1.669</v>
@@ -3846,7 +3846,7 @@
         <v>6.2199999999999998E-2</v>
       </c>
       <c r="AU17" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV17" s="1">
         <v>2.4900000000000002</v>
@@ -3855,48 +3855,48 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AX17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C18" s="1">
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O18" s="1">
         <v>1</v>
@@ -3953,10 +3953,10 @@
         <v>2</v>
       </c>
       <c r="AH18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ18" s="1">
         <v>0</v>
@@ -3969,10 +3969,10 @@
         <v>0.5</v>
       </c>
       <c r="AN18" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP18" s="1">
         <v>1</v>
@@ -3981,7 +3981,7 @@
         <v>0.1</v>
       </c>
       <c r="AR18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS18" s="1">
         <v>0.91720000000000002</v>
@@ -3990,7 +3990,7 @@
         <v>1.0359999999999999E-2</v>
       </c>
       <c r="AU18" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV18" s="1">
         <v>1</v>
@@ -3999,7 +3999,7 @@
         <v>0.1</v>
       </c>
       <c r="AX18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AY18" s="1">
         <v>0.91720000000000002</v>
@@ -4008,48 +4008,48 @@
         <v>1.0359999999999999E-2</v>
       </c>
       <c r="BA18" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C19" s="1">
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>102</v>
+        <v>215</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O19" s="1">
         <v>1</v>
@@ -4106,10 +4106,10 @@
         <v>2</v>
       </c>
       <c r="AH19" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ19" s="1">
         <v>0</v>
@@ -4122,10 +4122,10 @@
         <v>0.5</v>
       </c>
       <c r="AN19" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP19" s="1">
         <v>1</v>
@@ -4134,7 +4134,7 @@
         <v>0.1</v>
       </c>
       <c r="AR19" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS19" s="1">
         <v>1.03</v>
@@ -4143,7 +4143,7 @@
         <v>0.06</v>
       </c>
       <c r="AU19" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AV19" s="1">
         <v>0.74619999999999997</v>
@@ -4152,7 +4152,7 @@
         <v>1.55E-2</v>
       </c>
       <c r="AX19" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AY19" s="1">
         <v>0.74619999999999997</v>
@@ -4161,48 +4161,48 @@
         <v>1.55E-2</v>
       </c>
       <c r="BA19" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C20" s="1">
         <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O20" s="1">
         <v>1</v>
@@ -4259,10 +4259,10 @@
         <v>2</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ20" s="1">
         <v>0</v>
@@ -4275,10 +4275,10 @@
         <v>0.5</v>
       </c>
       <c r="AN20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP20" s="1">
         <v>1</v>
@@ -4287,7 +4287,7 @@
         <v>0.1</v>
       </c>
       <c r="AR20" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS20" s="1">
         <v>1.88</v>
@@ -4296,7 +4296,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AU20" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV20" s="1">
         <v>2.58</v>
@@ -4305,54 +4305,54 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AX20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AY20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA20" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AY20" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA20" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C21" s="1">
         <v>19</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O21" s="1">
         <v>1</v>
@@ -4409,10 +4409,10 @@
         <v>2</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ21" s="1">
         <v>0</v>
@@ -4425,10 +4425,10 @@
         <v>0.5</v>
       </c>
       <c r="AN21" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO21" s="2" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="AP21" s="1">
         <v>1</v>
@@ -4437,7 +4437,7 @@
         <v>0.1</v>
       </c>
       <c r="AR21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS21" s="1">
         <v>1.88</v>
@@ -4446,7 +4446,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AU21" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV21" s="1">
         <v>2.58</v>
@@ -4455,54 +4455,54 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AX21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AY21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA21" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AY21" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA21" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C22" s="1">
         <v>19</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O22" s="1">
         <v>1</v>
@@ -4559,10 +4559,10 @@
         <v>2</v>
       </c>
       <c r="AH22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ22" s="1">
         <v>0</v>
@@ -4575,10 +4575,10 @@
         <v>0.5</v>
       </c>
       <c r="AN22" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO22" s="2" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="AP22" s="1">
         <v>1</v>
@@ -4587,7 +4587,7 @@
         <v>0.1</v>
       </c>
       <c r="AR22" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS22" s="1">
         <v>1.88</v>
@@ -4596,7 +4596,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AU22" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV22" s="1">
         <v>2.58</v>
@@ -4605,54 +4605,54 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AX22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AY22" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA22" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AY22" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA22" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C23" s="1">
         <v>19</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O23" s="1">
         <v>1</v>
@@ -4709,10 +4709,10 @@
         <v>2</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ23" s="1">
         <v>0</v>
@@ -4725,10 +4725,10 @@
         <v>0.5</v>
       </c>
       <c r="AN23" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO23" s="2" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="AP23" s="1">
         <v>1</v>
@@ -4737,7 +4737,7 @@
         <v>0.1</v>
       </c>
       <c r="AR23" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS23" s="1">
         <v>1.88</v>
@@ -4746,7 +4746,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AU23" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV23" s="1">
         <v>2.58</v>
@@ -4755,21 +4755,21 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AX23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AY23" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA23" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AY23" s="1">
-        <v>1</v>
-      </c>
-      <c r="BA23" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C24" s="1">
         <v>20</v>
@@ -4778,31 +4778,31 @@
         <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="I24" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O24" s="1">
         <v>1</v>
@@ -4859,10 +4859,10 @@
         <v>2</v>
       </c>
       <c r="AH24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ24" s="1">
         <v>0</v>
@@ -4875,10 +4875,10 @@
         <v>0.5</v>
       </c>
       <c r="AN24" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP24" s="1">
         <v>1</v>
@@ -4887,7 +4887,7 @@
         <v>0.1</v>
       </c>
       <c r="AR24" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS24" s="1">
         <v>1</v>
@@ -4896,7 +4896,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AU24" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV24" s="1">
         <v>-0.01</v>
@@ -4905,27 +4905,27 @@
         <v>1E-3</v>
       </c>
       <c r="AX24" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AY24" s="4">
         <v>0.5</v>
       </c>
       <c r="BA24" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="BB24" s="1">
         <v>1000</v>
       </c>
       <c r="BD24" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="C25" s="1">
         <v>21</v>
@@ -4934,31 +4934,31 @@
         <v>21</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O25" s="1">
         <v>1</v>
@@ -5015,10 +5015,10 @@
         <v>2</v>
       </c>
       <c r="AH25" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ25" s="1">
         <v>0</v>
@@ -5031,10 +5031,10 @@
         <v>0.5</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP25" s="1">
         <v>1</v>
@@ -5043,13 +5043,13 @@
         <v>0.1</v>
       </c>
       <c r="AR25" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AS25" s="1">
         <v>-5</v>
       </c>
       <c r="AU25" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AV25" s="1">
         <v>1</v>
@@ -5058,27 +5058,27 @@
         <v>0.1</v>
       </c>
       <c r="AX25" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AY25" s="1">
         <v>1</v>
       </c>
       <c r="BA25" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="BB25" s="1">
         <v>300</v>
       </c>
       <c r="BD25" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C26" s="1">
         <v>22</v>
@@ -5087,31 +5087,31 @@
         <v>22</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O26" s="1">
         <v>1</v>
@@ -5168,10 +5168,10 @@
         <v>2</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI26" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ26" s="1">
         <v>0</v>
@@ -5184,10 +5184,10 @@
         <v>0.5</v>
       </c>
       <c r="AN26" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP26" s="1">
         <v>1</v>
@@ -5196,13 +5196,13 @@
         <v>0.1</v>
       </c>
       <c r="AR26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AS26" s="1">
         <v>-5</v>
       </c>
       <c r="AU26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AV26" s="1">
         <v>1</v>
@@ -5211,60 +5211,60 @@
         <v>0.1</v>
       </c>
       <c r="AX26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AY26" s="1">
         <v>1</v>
       </c>
       <c r="BA26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="BB26" s="1">
         <v>300</v>
       </c>
       <c r="BD26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C27" s="1">
         <v>11</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O27" s="1">
         <v>1</v>
@@ -5321,10 +5321,10 @@
         <v>2</v>
       </c>
       <c r="AH27" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ27" s="1">
         <v>0</v>
@@ -5337,10 +5337,10 @@
         <v>0.5</v>
       </c>
       <c r="AN27" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP27" s="4">
         <v>5.0199999999999996</v>
@@ -5349,7 +5349,7 @@
         <v>0.48</v>
       </c>
       <c r="AR27" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS27" s="1">
         <v>1.2989999999999999</v>
@@ -5358,48 +5358,48 @@
         <v>0.114</v>
       </c>
       <c r="AU27" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C28" s="1">
         <v>11</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O28" s="1">
         <v>1</v>
@@ -5456,10 +5456,10 @@
         <v>2</v>
       </c>
       <c r="AH28" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ28" s="1">
         <v>0</v>
@@ -5472,10 +5472,10 @@
         <v>0.5</v>
       </c>
       <c r="AN28" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP28" s="4">
         <v>5.0199999999999996</v>
@@ -5484,7 +5484,7 @@
         <v>0.48</v>
       </c>
       <c r="AR28" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS28" s="1">
         <v>1.399</v>
@@ -5493,48 +5493,48 @@
         <v>0.114</v>
       </c>
       <c r="AU28" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:56" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C29" s="1">
         <v>11</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O29" s="1">
         <v>1</v>
@@ -5591,10 +5591,10 @@
         <v>2</v>
       </c>
       <c r="AH29" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AI29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AJ29" s="1">
         <v>0</v>
@@ -5607,10 +5607,10 @@
         <v>0.5</v>
       </c>
       <c r="AN29" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AO29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AP29" s="4">
         <v>4.0199999999999996</v>
@@ -5619,7 +5619,7 @@
         <v>0.48</v>
       </c>
       <c r="AR29" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AS29" s="1">
         <v>1.1990000000000001</v>
@@ -5628,7 +5628,7 @@
         <v>0.114</v>
       </c>
       <c r="AU29" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>